<commit_message>
add another test case for ZSS-1384
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1384-overflow-right-align-frozen.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1384-overflow-right-align-frozen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zkspreadsheet/zss.test/src/main/webapp/issue3/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74D53A9-BA7B-9549-8451-D3C8C4CDACA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3283D690-4102-6B46-934F-D63FAA7B09C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37340" yWindow="840" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>a loooong text with left alingment</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>C11:D11 a merged cell with right alignment</t>
+  </si>
+  <si>
+    <t>B7 merged on left</t>
+  </si>
+  <si>
+    <t>D7 merged on data</t>
   </si>
 </sst>
 </file>
@@ -193,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -216,15 +222,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +516,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C12" sqref="C12"/>
+      <selection pane="topRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,23 +539,33 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="13"/>
+    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
       <c r="I10" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12" s="7" t="s">
@@ -566,9 +583,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -601,10 +620,10 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -662,10 +681,10 @@
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="11"/>
+      <c r="E11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="12"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D70" s="1" t="s">

</xml_diff>